<commit_message>
se sube ultima version de PC para Irina
</commit_message>
<xml_diff>
--- a/PCQA/ExcelAnulaciones.xlsx
+++ b/PCQA/ExcelAnulaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\DataSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78935A8C-28BE-4C23-BD34-7A6482C866BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98753D82-B1BA-488E-B6EA-6BEB797CAAC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>https://i-preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
   </si>
   <si>
-    <t>04104008320</t>
+    <t>12112001753</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Arreglos en los scripts de anulacion y rehabilitacion
</commit_message>
<xml_diff>
--- a/PCQA/ExcelAnulaciones.xlsx
+++ b/PCQA/ExcelAnulaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98753D82-B1BA-488E-B6EA-6BEB797CAAC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDAFDB4-3B07-4DC9-9E00-F414B67D872B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>NroPoliza</t>
   </si>
@@ -33,18 +33,9 @@
     <t>URL</t>
   </si>
   <si>
-    <t>ssurgwsoadev4.opc.oracleoutsourcing.com</t>
-  </si>
-  <si>
-    <t>https://ssurgwsoadev4.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
-  </si>
-  <si>
     <t>su</t>
   </si>
   <si>
-    <t>gw</t>
-  </si>
-  <si>
     <t>Usuario</t>
   </si>
   <si>
@@ -54,22 +45,13 @@
     <t>silverarrow</t>
   </si>
   <si>
-    <t>i-gestion-ssur-oci.opc.oracleoutsourcing.com</t>
-  </si>
-  <si>
-    <t>https://i-gestion-ssur-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
-  </si>
-  <si>
-    <t>suraqa</t>
-  </si>
-  <si>
     <t>i-preproducciongestion.segurossura.com.ar</t>
   </si>
   <si>
     <t>https://i-preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
   </si>
   <si>
-    <t>12112001753</t>
+    <t>04104013566</t>
   </si>
 </sst>
 </file>
@@ -469,7 +451,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,10 +469,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -498,57 +480,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3">
-        <v>11410004659</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>11111001337</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
@@ -557,11 +512,8 @@
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{0887811F-5A43-41A8-AFAC-9F62871E18A4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
agrego motivo de anulacion como variable en el DS y en el repositorio
</commit_message>
<xml_diff>
--- a/PCQA/ExcelAnulaciones.xlsx
+++ b/PCQA/ExcelAnulaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDAFDB4-3B07-4DC9-9E00-F414B67D872B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540AB668-D05A-44DF-9724-DFAD95E3485E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>NroPoliza</t>
   </si>
@@ -51,7 +51,13 @@
     <t>https://i-preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
   </si>
   <si>
-    <t>04104013566</t>
+    <t>OpcionMotivo</t>
+  </si>
+  <si>
+    <t>Anulación por desistimiento</t>
+  </si>
+  <si>
+    <t>12112001837</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +467,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -477,8 +483,11 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -492,23 +501,26 @@
         <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nueva rama para anulacion de poliza
</commit_message>
<xml_diff>
--- a/PCQA/ExcelAnulaciones.xlsx
+++ b/PCQA/ExcelAnulaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDAFDB4-3B07-4DC9-9E00-F414B67D872B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9499DEA-15E7-438E-BE21-5CD8B4A5FEE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>NroPoliza</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>04104013566</t>
+  </si>
+  <si>
+    <t>MotivoAnulacion</t>
+  </si>
+  <si>
+    <t>Anulación por Desistimiento</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +467,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -477,8 +483,11 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -494,21 +503,24 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifica data para empezar regresion R34 en Pre Prod
</commit_message>
<xml_diff>
--- a/PCQA/ExcelAnulaciones.xlsx
+++ b/PCQA/ExcelAnulaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540AB668-D05A-44DF-9724-DFAD95E3485E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CFE1F9-DBBA-4B5B-88AF-C269E35B0118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="37">
   <si>
     <t>NroPoliza</t>
   </si>
@@ -57,14 +57,89 @@
     <t>Anulación por desistimiento</t>
   </si>
   <si>
-    <t>12112001837</t>
+    <t>04104016436</t>
+  </si>
+  <si>
+    <t>04104016440</t>
+  </si>
+  <si>
+    <t>04104016443</t>
+  </si>
+  <si>
+    <t>04104016442</t>
+  </si>
+  <si>
+    <t>04104016441</t>
+  </si>
+  <si>
+    <t>04104016414</t>
+  </si>
+  <si>
+    <t>04104016461</t>
+  </si>
+  <si>
+    <t>04104016462</t>
+  </si>
+  <si>
+    <t>04104016463</t>
+  </si>
+  <si>
+    <t>04104016501</t>
+  </si>
+  <si>
+    <t>04104016464</t>
+  </si>
+  <si>
+    <t>11111003165</t>
+  </si>
+  <si>
+    <t>11111003167</t>
+  </si>
+  <si>
+    <t>12112001898</t>
+  </si>
+  <si>
+    <t>12112001899</t>
+  </si>
+  <si>
+    <t>12112001900</t>
+  </si>
+  <si>
+    <t>12112001903</t>
+  </si>
+  <si>
+    <t>12112001904</t>
+  </si>
+  <si>
+    <t>12112001905</t>
+  </si>
+  <si>
+    <t>04104016482</t>
+  </si>
+  <si>
+    <t>04104016483</t>
+  </si>
+  <si>
+    <t>04104016484</t>
+  </si>
+  <si>
+    <t>04104016485</t>
+  </si>
+  <si>
+    <t>04104016486</t>
+  </si>
+  <si>
+    <t>04104016434</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,13 +151,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,12 +177,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -454,74 +520,617 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>